<commit_message>
youtube.com checklist 28.02. 22:00
</commit_message>
<xml_diff>
--- a/googlevideo.com domains/Mappe1.xlsx
+++ b/googlevideo.com domains/Mappe1.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$A$768</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$A$779</definedName>
     <definedName name="_xlnm.Extract" localSheetId="0">Tabelle1!$C:$C</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="95">
   <si>
     <t>advertisment</t>
   </si>
@@ -249,12 +249,12 @@
     <t>r1---sn-p5qlsnsd.googlevideo.com</t>
   </si>
   <si>
+    <t>r5---sn-4g5e6ney.googlevideo.com</t>
+  </si>
+  <si>
     <t>r3---sn-4g5e6nez.googlevideo.com</t>
   </si>
   <si>
-    <t>r5---sn-4g5e6ney.googlevideo.com #2x</t>
-  </si>
-  <si>
     <t>r2---sn-4g5e6n7d.googlevideo.com</t>
   </si>
   <si>
@@ -277,6 +277,42 @@
   </si>
   <si>
     <t>r16---sn-4g57knl7.googlevideo.com</t>
+  </si>
+  <si>
+    <t>r1---sn-4g57knrl.googlevideo.com</t>
+  </si>
+  <si>
+    <t>r4---sn-5hnednlk.googlevideo.com</t>
+  </si>
+  <si>
+    <t>r20---sn-5hne6n76.googlevideo.com</t>
+  </si>
+  <si>
+    <t>r10---sn-4g57knke.googlevideo.com</t>
+  </si>
+  <si>
+    <t>r4---sn-5hne6n7r.googlevideo.com</t>
+  </si>
+  <si>
+    <t>r6---sn-5hne6nlr.googlevideo.com</t>
+  </si>
+  <si>
+    <t>r11---sn-a5m7znes.googlevideo.com</t>
+  </si>
+  <si>
+    <t>r5---sn-4g5e6ne6.googlevideo.com</t>
+  </si>
+  <si>
+    <t>r2---sn-5hne6n7z.googlevideo.com</t>
+  </si>
+  <si>
+    <t>r5---sn-a5meknek.googlevideo.com</t>
+  </si>
+  <si>
+    <t>r5---sn-4g57knzl.googlevideo.com</t>
+  </si>
+  <si>
+    <t>r2---sn-4g5ednll.googlevideo.com</t>
   </si>
 </sst>
 </file>
@@ -636,17 +672,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D768"/>
+  <dimension ref="A1:D779"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="L52" sqref="L52"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="40.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="40.453125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.26953125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="10.90625" style="2" customWidth="1"/>
     <col min="9" max="16384" width="10.90625" style="2"/>
@@ -693,22 +727,22 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -718,417 +752,431 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B14" s="2" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C14" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C15" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C17" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C18" s="1" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B21" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B22" s="2" t="s">
-        <v>5</v>
+      <c r="A22" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B23" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B24" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B25" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C24" s="1" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C26" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C27" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B27" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B28" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B29" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B30" s="2" t="s">
-        <v>73</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B31" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B32" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B33" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B34" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C32" s="1" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C35" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C33" s="1" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C36" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C34" s="1" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C37" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B36" s="2" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B40" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B37" s="2" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B41" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C38" s="1" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C42" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C39" s="1" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C43" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C44" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C40" s="1" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C45" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C41" s="1" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C46" s="1" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B43" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B44" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B48" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B49" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B50" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B51" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C52" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" s="1"/>
-      <c r="B48" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" s="1"/>
-      <c r="B49" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" s="1"/>
-      <c r="B50" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C51" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C52" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C53" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C54" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C55" s="1"/>
-      <c r="D55" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C57" s="1" t="s">
-        <v>27</v>
+      <c r="A57" s="1"/>
+      <c r="B57" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C58" s="1" t="s">
-        <v>36</v>
+      <c r="A58" s="1"/>
+      <c r="B58" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A59" s="1" t="s">
-        <v>59</v>
+      <c r="A59" s="1"/>
+      <c r="B59" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A60" s="1" t="s">
-        <v>48</v>
+      <c r="C60" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B61" s="1" t="s">
-        <v>40</v>
+      <c r="C61" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C62" s="1" t="s">
-        <v>76</v>
+        <v>25</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C63" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C64" s="1" t="s">
-        <v>64</v>
+      <c r="C64" s="1"/>
+      <c r="D64" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B65" s="2" t="s">
-        <v>69</v>
+      <c r="A65" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B66" s="2" t="s">
-        <v>16</v>
+      <c r="C66" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C67" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B68" s="2" t="s">
-        <v>50</v>
+      <c r="A68" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C69" s="1" t="s">
-        <v>29</v>
+      <c r="A69" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C70" s="1" t="s">
-        <v>41</v>
+      <c r="B70" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B71" s="2" t="s">
-        <v>17</v>
+      <c r="C71" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B72" s="2" t="s">
-        <v>82</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="C72" s="1"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B73" s="2" t="s">
-        <v>18</v>
+      <c r="C73" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A74" s="1" t="s">
-        <v>43</v>
+      <c r="C74" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B75" s="2" t="s">
-        <v>61</v>
+      <c r="C75" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B76" s="2" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C77" s="1" t="s">
-        <v>30</v>
+      <c r="B77" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B78" s="2" t="s">
-        <v>19</v>
+      <c r="C78" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C79" s="1" t="s">
-        <v>31</v>
+      <c r="B79" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B80" s="2" t="s">
-        <v>78</v>
+      <c r="C80" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C81" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B82" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B83" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B84" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B86" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B87" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C88" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B89" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C90" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B91" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C92" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C82" s="1" t="s">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C93" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C83" s="1" t="s">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C94" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A84" s="1"/>
-      <c r="C84" s="1"/>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A85" s="1"/>
-      <c r="C85" s="1"/>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A86" s="1"/>
-      <c r="C86" s="1"/>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A87" s="1"/>
-      <c r="C87" s="1"/>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A88" s="1"/>
-      <c r="C88" s="1"/>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A89" s="1"/>
-      <c r="C89" s="1"/>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A90" s="1"/>
-      <c r="C90" s="1"/>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A91" s="1"/>
-      <c r="C91" s="1"/>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A92" s="1"/>
-      <c r="C92" s="1"/>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A93" s="1"/>
-      <c r="C93" s="1"/>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A94" s="1"/>
-      <c r="C94" s="1"/>
-    </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A95" s="1"/>
+      <c r="A95" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="C95" s="1"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
@@ -3823,9 +3871,53 @@
       <c r="A768" s="1"/>
       <c r="C768" s="1"/>
     </row>
+    <row r="769" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A769" s="1"/>
+      <c r="C769" s="1"/>
+    </row>
+    <row r="770" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A770" s="1"/>
+      <c r="C770" s="1"/>
+    </row>
+    <row r="771" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A771" s="1"/>
+      <c r="C771" s="1"/>
+    </row>
+    <row r="772" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A772" s="1"/>
+      <c r="C772" s="1"/>
+    </row>
+    <row r="773" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A773" s="1"/>
+      <c r="C773" s="1"/>
+    </row>
+    <row r="774" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A774" s="1"/>
+      <c r="C774" s="1"/>
+    </row>
+    <row r="775" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A775" s="1"/>
+      <c r="C775" s="1"/>
+    </row>
+    <row r="776" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A776" s="1"/>
+      <c r="C776" s="1"/>
+    </row>
+    <row r="777" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A777" s="1"/>
+      <c r="C777" s="1"/>
+    </row>
+    <row r="778" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A778" s="1"/>
+      <c r="C778" s="1"/>
+    </row>
+    <row r="779" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A779" s="1"/>
+      <c r="C779" s="1"/>
+    </row>
   </sheetData>
-  <sortState ref="C81:C83">
-    <sortCondition ref="C81"/>
+  <sortState ref="A53:A56">
+    <sortCondition ref="A56"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>